<commit_message>
Site updated: 2021-04-13 17:46:00
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -26,6 +26,45 @@
   </si>
   <si>
     <t>|||</t>
+  </si>
+  <si>
+    <t>三角形</t>
+  </si>
+  <si>
+    <t>||</t>
+  </si>
+  <si>
+    <t>比较典型的动态规划题，可看一看</t>
+  </si>
+  <si>
+    <t>买卖股票的最佳时机</t>
+  </si>
+  <si>
+    <t>感觉思路也不是很好想</t>
+  </si>
+  <si>
+    <t>买卖股票的最佳时机||</t>
+  </si>
+  <si>
+    <t>验证回形串</t>
+  </si>
+  <si>
+    <t>字符串比较操作要会，思路简单</t>
+  </si>
+  <si>
+    <t>分割回文串</t>
+  </si>
+  <si>
+    <t>||||</t>
+  </si>
+  <si>
+    <t>回溯问题，要看！</t>
+  </si>
+  <si>
+    <t>克隆图</t>
+  </si>
+  <si>
+    <t>图的dfs和bfs遍历，要看！</t>
   </si>
 </sst>
 </file>
@@ -34,8 +73,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -48,7 +87,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -61,24 +122,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -86,22 +132,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,14 +145,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -131,8 +153,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,9 +168,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,22 +201,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,55 +239,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,7 +383,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +407,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,103 +419,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,15 +430,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -428,16 +458,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -446,17 +476,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -478,16 +497,36 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,148 +535,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -964,13 +1003,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
+  <cols>
+    <col min="3" max="3" width="17.0833333333333" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2">
@@ -992,6 +1034,97 @@
       </c>
       <c r="D3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2021-04-16 16:38:44
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>图的dfs和bfs遍历，要看！</t>
+  </si>
+  <si>
+    <t>只出现一次的数字||</t>
+  </si>
+  <si>
+    <t>位运算相关，比较新颖的做法</t>
+  </si>
+  <si>
+    <t>复制带随机指针的链表</t>
+  </si>
+  <si>
+    <t>背一下这个套路，套路类似于133题</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1015,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E13"/>
+  <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
@@ -1127,6 +1139,48 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-04-17 12:08:21
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13460"/>
+    <workbookView windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>背一下这个套路，套路类似于133题</t>
+  </si>
+  <si>
+    <t>拆分词句</t>
+  </si>
+  <si>
+    <t>可以用动态规划，也可以用回溯，比较经典</t>
+  </si>
+  <si>
+    <t>单链表中的环</t>
+  </si>
+  <si>
+    <t>快慢指针，用了比较巧妙的方法</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1027,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E18"/>
+  <dimension ref="A2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
@@ -1181,6 +1193,34 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-04-20 11:05:33
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -89,6 +89,27 @@
   </si>
   <si>
     <t>快慢指针，用了比较巧妙的方法</t>
+  </si>
+  <si>
+    <t>单链表中的环2</t>
+  </si>
+  <si>
+    <t>同上一题差不多</t>
+  </si>
+  <si>
+    <t>重排链表</t>
+  </si>
+  <si>
+    <t>不是很难</t>
+  </si>
+  <si>
+    <t>树的前序遍历</t>
+  </si>
+  <si>
+    <t>树的后续遍历</t>
+  </si>
+  <si>
+    <t>迭代法一定要会！！！</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1048,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E21"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
@@ -1221,6 +1242,59 @@
         <v>24</v>
       </c>
     </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>142</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>143</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-04-26 20:28:29
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -110,6 +110,30 @@
   </si>
   <si>
     <t>迭代法一定要会！！！</t>
+  </si>
+  <si>
+    <t>排序链表</t>
+  </si>
+  <si>
+    <t>|||||</t>
+  </si>
+  <si>
+    <t>分治算法，用到了递归，以前没有写过分治，要看！</t>
+  </si>
+  <si>
+    <t>翻转字符串里的单词</t>
+  </si>
+  <si>
+    <t>乘积最大子数组</t>
+  </si>
+  <si>
+    <t>动态规划法，比较奇怪的思路</t>
+  </si>
+  <si>
+    <t>寻找旋转排序数组中的最小值</t>
+  </si>
+  <si>
+    <t>经典二分查找变形题，自己做出来了</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1072,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E25"/>
+  <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
@@ -1295,6 +1319,59 @@
         <v>31</v>
       </c>
     </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>148</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>152</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>153</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-04-27 10:11:51
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>经典二分查找变形题，自己做出来了</t>
+  </si>
+  <si>
+    <t>相交链表</t>
+  </si>
+  <si>
+    <t>思路可以看一下，没做出来</t>
+  </si>
+  <si>
+    <t>寻找峰值</t>
+  </si>
+  <si>
+    <t>挺简单的，做出来了</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1084,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E31"/>
+  <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
@@ -1372,6 +1384,34 @@
         <v>39</v>
       </c>
     </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>160</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>162</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-04-29 11:37:53
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>挺简单的，做出来了</t>
+  </si>
+  <si>
+    <t>比较版本号</t>
+  </si>
+  <si>
+    <t>思路简单</t>
+  </si>
+  <si>
+    <t>分数到小数</t>
+  </si>
+  <si>
+    <t>不擅长这种题目，要看一看</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1096,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E40"/>
+  <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
@@ -1412,6 +1424,34 @@
         <v>43</v>
       </c>
     </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>165</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>166</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-05-06 17:10:38
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>不擅长这种题目，要看一看</t>
+  </si>
+  <si>
+    <t>两数之和，有序版</t>
+  </si>
+  <si>
+    <t>可以用二分查找或者双指针，双指针方法要会</t>
+  </si>
+  <si>
+    <t>Excel表列名称</t>
+  </si>
+  <si>
+    <t>糟心的数学相关题</t>
   </si>
 </sst>
 </file>
@@ -165,10 +177,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -179,6 +191,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -186,45 +206,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,6 +228,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -246,71 +298,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,37 +344,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,145 +524,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,36 +543,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,6 +567,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,153 +620,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1096,10 +1108,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E44"/>
+  <dimension ref="A2:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
@@ -1452,6 +1464,34 @@
         <v>47</v>
       </c>
     </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>167</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>168</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-05-11 21:28:07
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13200"/>
+    <workbookView windowWidth="28800" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -170,6 +170,45 @@
   </si>
   <si>
     <t>糟心的数学相关题</t>
+  </si>
+  <si>
+    <t>多数元素</t>
+  </si>
+  <si>
+    <t>解法很多</t>
+  </si>
+  <si>
+    <t>Excel表列序号</t>
+  </si>
+  <si>
+    <t>联系168一起看</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array||</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>Median of Two Sorted Arrays</t>
   </si>
 </sst>
 </file>
@@ -182,10 +221,31 @@
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -335,7 +395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +404,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -422,12 +506,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -441,12 +519,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,153 +712,183 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1108,13 +1210,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E46"/>
+  <dimension ref="A2:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="5"/>
   <cols>
     <col min="3" max="3" width="17.0833333333333" customWidth="1"/>
   </cols>
@@ -1492,6 +1594,104 @@
         <v>51</v>
       </c>
     </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>169</v>
+      </c>
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>171</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" t="s">
+        <v>58</v>
+      </c>
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" s="1" customFormat="1" spans="1:1">
+      <c r="A52" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" s="2" customFormat="1" spans="1:4">
+      <c r="A53" s="2">
+        <v>704</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" s="3" customFormat="1" spans="1:2">
+      <c r="A54" s="3">
+        <v>34</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" s="4" customFormat="1" spans="1:2">
+      <c r="A55" s="4">
+        <v>33</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" s="4" customFormat="1" spans="1:2">
+      <c r="A56" s="4">
+        <v>81</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" s="4" customFormat="1" spans="1:2">
+      <c r="A57" s="4">
+        <v>74</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" s="3" customFormat="1" spans="1:2">
+      <c r="A58" s="3">
+        <v>4</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-05-14 22:33:00
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13460"/>
+    <workbookView windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -209,6 +209,27 @@
   </si>
   <si>
     <t>Median of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t>Find the Smallest Divisor Given a Threshold</t>
+  </si>
+  <si>
+    <t>Multi Pointers</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Sort an Array(Quick Sort and Merge Sort)</t>
+  </si>
+  <si>
+    <t>Sort Colors</t>
+  </si>
+  <si>
+    <t>two pointers的方法还没看懂</t>
   </si>
 </sst>
 </file>
@@ -216,12 +237,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +269,89 @@
       <color theme="8"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -259,38 +363,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,97 +422,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -428,175 +456,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,47 +641,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -687,8 +676,32 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,153 +720,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -873,19 +901,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1210,10 +1238,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:F58"/>
+  <dimension ref="A2:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="5"/>
@@ -1626,11 +1654,11 @@
       <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="5"/>
+      <c r="B51" s="7"/>
       <c r="C51" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="6"/>
+      <c r="D51" s="8"/>
       <c r="E51" t="s">
         <v>58</v>
       </c>
@@ -1645,10 +1673,10 @@
       <c r="A53" s="2">
         <v>704</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1656,7 +1684,7 @@
       <c r="A54" s="3">
         <v>34</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1664,7 +1692,7 @@
       <c r="A55" s="4">
         <v>33</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1672,7 +1700,7 @@
       <c r="A56" s="4">
         <v>81</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1680,7 +1708,7 @@
       <c r="A57" s="4">
         <v>74</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1688,8 +1716,53 @@
       <c r="A58" s="3">
         <v>4</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="3" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="59" s="5" customFormat="1" spans="1:2">
+      <c r="A59" s="5">
+        <v>875</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" s="5" customFormat="1" spans="1:2">
+      <c r="A60" s="5">
+        <v>1283</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" s="1" customFormat="1" spans="1:1">
+      <c r="A62" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" s="6" customFormat="1" spans="1:2">
+      <c r="A64" s="6">
+        <v>912</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" s="5" customFormat="1" spans="1:5">
+      <c r="A65" s="5">
+        <v>75</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2021-05-17 21:14:10
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -230,6 +230,18 @@
   </si>
   <si>
     <t>two pointers的方法还没看懂</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array ||</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>Move Zeros</t>
   </si>
 </sst>
 </file>
@@ -1238,10 +1250,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:F65"/>
+  <dimension ref="A2:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="5"/>
@@ -1765,6 +1777,38 @@
         <v>71</v>
       </c>
     </row>
+    <row r="66" s="6" customFormat="1" spans="1:2">
+      <c r="A66" s="6">
+        <v>26</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" s="5" customFormat="1" spans="1:2">
+      <c r="A67" s="5">
+        <v>80</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" s="5" customFormat="1" spans="1:2">
+      <c r="A68" s="5">
+        <v>88</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" s="5" customFormat="1" spans="1:2">
+      <c r="A69" s="5">
+        <v>283</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2021-10-14 14:32:51
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13200"/>
+    <workbookView windowWidth="28480" windowHeight="12820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,9 +249,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -305,6 +305,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -313,16 +382,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,92 +407,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -434,6 +420,20 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -468,19 +468,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,13 +546,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,19 +600,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,109 +618,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,16 +660,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,11 +685,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,37 +734,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -752,152 +752,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -916,16 +916,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1252,8 +1246,8 @@
   <sheetPr/>
   <dimension ref="A2:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="5"/>
@@ -1666,15 +1660,15 @@
       <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
       <c r="C51" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="8"/>
+      <c r="D51" s="7"/>
       <c r="E51" t="s">
         <v>58</v>
       </c>
-      <c r="F51" s="10"/>
+      <c r="F51" s="8"/>
     </row>
     <row r="52" s="1" customFormat="1" spans="1:1">
       <c r="A52" s="1" t="s">
@@ -1736,7 +1730,7 @@
       <c r="A59" s="5">
         <v>875</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1744,7 +1738,7 @@
       <c r="A60" s="5">
         <v>1283</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1758,8 +1752,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" s="6" customFormat="1" spans="1:2">
-      <c r="A64" s="6">
+    <row r="64" s="2" customFormat="1" spans="1:2">
+      <c r="A64" s="2">
         <v>912</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -1770,15 +1764,15 @@
       <c r="A65" s="5">
         <v>75</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" s="6" customFormat="1" spans="1:2">
-      <c r="A66" s="6">
+    <row r="66" s="2" customFormat="1" spans="1:2">
+      <c r="A66" s="2">
         <v>26</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -1789,7 +1783,7 @@
       <c r="A67" s="5">
         <v>80</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1797,7 +1791,7 @@
       <c r="A68" s="5">
         <v>88</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1805,7 +1799,7 @@
       <c r="A69" s="5">
         <v>283</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="5" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Site updated: 2022-01-06 12:33:48
</commit_message>
<xml_diff>
--- a/Leetcode难度梳理.xlsx
+++ b/Leetcode难度梳理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28480" windowHeight="12820"/>
+    <workbookView windowWidth="28480" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114">
   <si>
     <t>杨辉三角</t>
   </si>
@@ -242,6 +242,140 @@
   </si>
   <si>
     <t>Move Zeros</t>
+  </si>
+  <si>
+    <t>Facebook Tag</t>
+  </si>
+  <si>
+    <t>56.Merge Intervals</t>
+  </si>
+  <si>
+    <t>sort，判断后一个interval的前边界是否&lt;=前一个interval的后边界</t>
+  </si>
+  <si>
+    <t>42.Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>Stack，用while循环，遇到上升边缘，st.pop()前一个低谷，之后和st.top()比较计算res</t>
+  </si>
+  <si>
+    <t>560.Subarray Sum Equals K</t>
+  </si>
+  <si>
+    <t>计算sum，利用hash表记录遍历道第i个元素，sum-k的个数。</t>
+  </si>
+  <si>
+    <t>1249.Minimum Remove to Make Valid Parenthese</t>
+  </si>
+  <si>
+    <t>stack中只存储）的index，若(数量&gt;(数量，则要删除;若最终stack中还剩（则要删除。注意，诀窍是在遍历过程中标记需要删除的括号为*，最后统一遍历一遍string，求出res</t>
+  </si>
+  <si>
+    <t>31. Next Permutation</t>
+  </si>
+  <si>
+    <t>右到左找到第一个prev&lt;after的元素，设其index为i。在从右到左，i+1-nums.size()-1中找到第一个比prev大的元素，与prev交换。reverse i+1-nums.size()-1区间的元素。</t>
+  </si>
+  <si>
+    <t>215. Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>973. K Closest Points to Origin</t>
+  </si>
+  <si>
+    <t>注意是距离最近的k个点，使用priority_queue排序，并却在q.size()&gt;k时，进行q.pop()，滤去更大的元素</t>
+  </si>
+  <si>
+    <t>680. Valid Palindrome ||</t>
+  </si>
+  <si>
+    <t>408. Valid Word Abbreviation</t>
+  </si>
+  <si>
+    <t>two pointers，注意处理数字的方式</t>
+  </si>
+  <si>
+    <t>1382. Balance a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>（1）Inorder遍历，得有序node vector （2）递归，每次取中点作为root，构成平衡搜索二叉树</t>
+  </si>
+  <si>
+    <t>1428. Leftmost Column with at Least a One</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 法一：每行binary search，找到第一个1，注意若该行最后一个元素为0，直接continue  法二：指针ptr从右上角开始，当前元素为1，则向左，直到不能向左，则向下。</t>
+  </si>
+  <si>
+    <t>1570. Dot Product of Two Sparse Vectors</t>
+  </si>
+  <si>
+    <t>hash表存储非0的index和value</t>
+  </si>
+  <si>
+    <t>1650. Lowest Common Ancestor of a Binary Tree |||</t>
+  </si>
+  <si>
+    <t>从node p开始找parent，直到找到root，将p～root的节点全部存储在hash map中；从node q开始找parent，直到找到hash map中已有的节点。此节点极为lowest ancestor</t>
+  </si>
+  <si>
+    <t>1762. Building With an Ocean View</t>
+  </si>
+  <si>
+    <t>倒序遍历array，若curr &gt; res.back()，则将curr加入res。因为最后加入res的元素，一定是curr-array.size()-1中最大的元素，如果curr大于最大的元素，则为海景房</t>
+  </si>
+  <si>
+    <r>
+      <t>314.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <rFont val="PingFang SC"/>
+        <charset val="134"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <rFont val="PingFang SC"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Binary Tree Vertical Order Traversal</t>
+    </r>
+  </si>
+  <si>
+    <t>BFS方法+treemap</t>
+  </si>
+  <si>
+    <t>398. Random Pick Index</t>
+  </si>
+  <si>
+    <t>char直接加string会报错：res = (sum % 10 + '0') + res;。res.insert(res.begin(), sum % 10 + '0');</t>
+  </si>
+  <si>
+    <t>415. Add Strings</t>
+  </si>
+  <si>
+    <t>523. Continuous Subarray Sum</t>
+  </si>
+  <si>
+    <t>若a%k = c, b%k = c, 则(a-b) % c = 0</t>
+  </si>
+  <si>
+    <t>543. Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>一个形参用来计算res，一个返回类型用来计算当前max</t>
+  </si>
+  <si>
+    <t>536. Construct Binary Tree from String</t>
+  </si>
+  <si>
+    <t>递归按照从大到小的思想，通过括号分出当下的左子树以及当下的右子树</t>
   </si>
 </sst>
 </file>
@@ -249,12 +383,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -291,6 +425,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -299,21 +455,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,8 +492,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -342,6 +546,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -349,91 +575,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -450,19 +591,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,13 +681,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,151 +753,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,8 +794,37 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,17 +840,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,21 +860,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -730,20 +874,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -752,152 +893,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -916,13 +1057,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1244,14 +1391,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:F69"/>
+  <dimension ref="A2:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="5"/>
   <cols>
+    <col min="1" max="1" width="59.3" customWidth="1"/>
     <col min="3" max="3" width="17.0833333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1660,15 +1808,15 @@
       <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="8"/>
       <c r="C51" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="7"/>
+      <c r="D51" s="6"/>
       <c r="E51" t="s">
         <v>58</v>
       </c>
-      <c r="F51" s="8"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" s="1" customFormat="1" spans="1:1">
       <c r="A52" s="1" t="s">
@@ -1801,6 +1949,162 @@
       </c>
       <c r="B69" s="5" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="75" s="6" customFormat="1" spans="1:1">
+      <c r="A75" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" s="7" customFormat="1" spans="1:4">
+      <c r="A77" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>85</v>
+      </c>
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="D82" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="D84" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>95</v>
+      </c>
+      <c r="D86" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>97</v>
+      </c>
+      <c r="D87" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>101</v>
+      </c>
+      <c r="D89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" ht="14" spans="1:4">
+      <c r="A90" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D90" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>105</v>
+      </c>
+      <c r="D91" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>108</v>
+      </c>
+      <c r="D93" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" s="7" customFormat="1" spans="1:4">
+      <c r="A94" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="95" s="7" customFormat="1" spans="1:4">
+      <c r="A95" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>